<commit_message>
done for now not tested with full team scouting
</commit_message>
<xml_diff>
--- a/output_data.xlsx
+++ b/output_data.xlsx
@@ -10,13 +10,14 @@
     <sheet name="Rankings" sheetId="1" r:id="rId1"/>
     <sheet name="Accuracy" sheetId="2" r:id="rId2"/>
     <sheet name="695" sheetId="3" r:id="rId3"/>
+    <sheet name="1787" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
   <si>
     <t>Ranks</t>
   </si>
@@ -70,6 +71,9 @@
   </si>
   <si>
     <t>Tank</t>
+  </si>
+  <si>
+    <t>Swerve</t>
   </si>
 </sst>
 </file>
@@ -510,4 +514,93 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>